<commit_message>
final grouping method fulfill
</commit_message>
<xml_diff>
--- a/server/files/download/SelectedResult.xlsx
+++ b/server/files/download/SelectedResult.xlsx
@@ -372,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D98"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -418,212 +418,212 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>邓赵红</v>
+        <v>张得天</v>
       </c>
       <c r="B4" t="str">
-        <v>安卓平台人类特征识别软件开发</v>
+        <v>基于微信公众号的搜索平台设计与实现</v>
       </c>
       <c r="C4" t="str">
-        <v>1030513111</v>
+        <v>1030513325</v>
       </c>
       <c r="D4" t="str">
-        <v>龙仕清</v>
+        <v>宋旭飞</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>陈飞</v>
+        <v>赵燕</v>
       </c>
       <c r="B5" t="str">
-        <v>微信小程序开发</v>
+        <v>三维动画设计</v>
       </c>
       <c r="C5" t="str">
-        <v>1030513231</v>
+        <v>1030513331</v>
       </c>
       <c r="D5" t="str">
-        <v>许军</v>
+        <v>吴若宇</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>赵燕</v>
+        <v>晏涛</v>
       </c>
       <c r="B6" t="str">
-        <v>基于VR技术的交互设计</v>
+        <v>基于图像的船型识别方法研究</v>
       </c>
       <c r="C6" t="str">
-        <v>1030513316</v>
+        <v>1030513414</v>
       </c>
       <c r="D6" t="str">
-        <v>王君临</v>
+        <v>林瑞</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>张得天</v>
+        <v>陈伟</v>
       </c>
       <c r="B7" t="str">
-        <v>垂直爬虫开发</v>
+        <v>魔方拼图</v>
       </c>
       <c r="C7" t="str">
-        <v>1030513332</v>
+        <v>1030513125</v>
       </c>
       <c r="D7" t="str">
-        <v>肖山民</v>
+        <v>刘俊</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>张得天</v>
+        <v>钱鹏江</v>
       </c>
       <c r="B8" t="str">
-        <v>基于微信公众号的搜索平台设计与实现</v>
+        <v>本科毕业设计管理系统设计与实现</v>
       </c>
       <c r="C8" t="str">
-        <v>1030513325</v>
+        <v>1030513425</v>
       </c>
       <c r="D8" t="str">
-        <v>宋旭飞</v>
+        <v>郭震方</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>张军</v>
+        <v>孟磊</v>
       </c>
       <c r="B9" t="str">
-        <v>基于真实云景照片的天空盒子纹理合成组件开发</v>
+        <v>后工业语境下的数字技术与文化遗产整合应用方法探析</v>
       </c>
       <c r="C9" t="str">
-        <v>1030513133</v>
+        <v>1030513202</v>
       </c>
       <c r="D9" t="str">
-        <v>庄蒙周</v>
+        <v>杜倩倩</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>张得天</v>
+        <v>钱鹏江</v>
       </c>
       <c r="B10" t="str">
-        <v>基于企业数据的爬虫</v>
+        <v>MapReduce分布式计算架构分析与实践</v>
       </c>
       <c r="C10" t="str">
-        <v>1030513129</v>
+        <v>1030513420</v>
       </c>
       <c r="D10" t="str">
-        <v>王斌</v>
+        <v>杨艺</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>蒋亦樟</v>
+        <v>律睿敏</v>
       </c>
       <c r="B11" t="str">
-        <v>基于智能方法的癫痫脑电信号识别研究</v>
+        <v>具有音频编辑与分享功能的音乐播放器开发</v>
       </c>
       <c r="C11" t="str">
-        <v>1030513208</v>
+        <v>1030513232</v>
       </c>
       <c r="D11" t="str">
-        <v>卢虹羽</v>
+        <v>杨笑寒</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>蒋亦樟</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B12" t="str">
-        <v>小区物业管理系统的设计与实现</v>
+        <v>基于html5的移动应用开发</v>
       </c>
       <c r="C12" t="str">
-        <v>1030513218</v>
+        <v>1030513319</v>
       </c>
       <c r="D12" t="str">
-        <v>朱静</v>
+        <v>赵欢</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>夏鸿斌</v>
+        <v>律睿敏</v>
       </c>
       <c r="B13" t="str">
-        <v>基于html5的移动应用开发</v>
+        <v>绘画解密游戏设计</v>
       </c>
       <c r="C13" t="str">
-        <v>1030513319</v>
+        <v>1030513122</v>
       </c>
       <c r="D13" t="str">
-        <v>赵欢</v>
+        <v>金振阳</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>刘渊</v>
+        <v>律睿敏</v>
       </c>
       <c r="B14" t="str">
-        <v>基于视频信息的测量与计算技术的研究</v>
+        <v>“六合棋”的人机对战AI算法设计</v>
       </c>
       <c r="C14" t="str">
-        <v>1030513233</v>
+        <v>1030513222</v>
       </c>
       <c r="D14" t="str">
-        <v>郑雨杰</v>
+        <v>李嘉文</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>张军</v>
+        <v>律睿敏</v>
       </c>
       <c r="B15" t="str">
-        <v>基于DirectX的全局光照算法SVO的框架软件开发</v>
+        <v>基于“六合棋”规则的解密类游戏开发</v>
       </c>
       <c r="C15" t="str">
-        <v>1030513408</v>
+        <v>1030513422</v>
       </c>
       <c r="D15" t="str">
-        <v>华清沁</v>
+        <v>白小山</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>张得天</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B16" t="str">
-        <v>欺诈短信的数据挖掘</v>
+        <v>视频目标跟踪方法研究与实现</v>
       </c>
       <c r="C16" t="str">
-        <v>1030513321</v>
+        <v>1030512302</v>
       </c>
       <c r="D16" t="str">
-        <v>葛亮</v>
+        <v>方旭</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>蒋亦樟</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B17" t="str">
-        <v>旅行社信息管理系统的设计与实现</v>
+        <v>与艺术性合作：基于unity交互引擎的数字艺术表现(章立)</v>
       </c>
       <c r="C17" t="str">
-        <v>1030513205</v>
+        <v>1030513314</v>
       </c>
       <c r="D17" t="str">
-        <v>刘孟楠</v>
+        <v>史罗琼</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>谢振平</v>
+        <v>张得天</v>
       </c>
       <c r="B18" t="str">
-        <v>大数据行为特征智能挖掘技术研究</v>
+        <v>欺诈短信的数据挖掘</v>
       </c>
       <c r="C18" t="str">
-        <v>1030513101</v>
+        <v>1030513321</v>
       </c>
       <c r="D18" t="str">
-        <v>陈梅婕</v>
+        <v>葛亮</v>
       </c>
     </row>
     <row r="19">
@@ -631,69 +631,69 @@
         <v>夏鸿斌</v>
       </c>
       <c r="B19" t="str">
-        <v>与艺术性合作：基于unity交互引擎的数字艺术表现(章立)</v>
+        <v>基于用户行为的电影推荐系统构建</v>
       </c>
       <c r="C19" t="str">
-        <v>1030513314</v>
+        <v>1030513213</v>
       </c>
       <c r="D19" t="str">
-        <v>史罗琼</v>
+        <v>徐慧敏</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>蒋亦樟</v>
+        <v>晏涛</v>
       </c>
       <c r="B20" t="str">
-        <v>面向甲状腺癌诊断的智能识别技术探索</v>
+        <v>多视点图像新视点生成技术研究</v>
       </c>
       <c r="C20" t="str">
-        <v>1030513415</v>
+        <v>1030513328</v>
       </c>
       <c r="D20" t="str">
-        <v>刘英姿</v>
+        <v>王家麟</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>谢振平</v>
+        <v>张得天</v>
       </c>
       <c r="B21" t="str">
-        <v>基于监控视频的会展人流特征分析及可视化</v>
+        <v>垂直爬虫开发</v>
       </c>
       <c r="C21" t="str">
-        <v>1030513429</v>
+        <v>1030513332</v>
       </c>
       <c r="D21" t="str">
-        <v>王伟林</v>
+        <v>肖山民</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>吴锋</v>
+        <v>陈飞</v>
       </c>
       <c r="B22" t="str">
-        <v>境外媒体对中国高铁的报道监测及数据可视化分析</v>
+        <v>基于ffmpeg的视频应用开发</v>
       </c>
       <c r="C22" t="str">
-        <v>1030513105</v>
+        <v>1030513126</v>
       </c>
       <c r="D22" t="str">
-        <v>郭越</v>
+        <v>沈苏明</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>陈飞</v>
+        <v>谢振平</v>
       </c>
       <c r="B23" t="str">
-        <v>基于ffmpeg的视频应用开发</v>
+        <v>大数据行为特征智能挖掘技术研究</v>
       </c>
       <c r="C23" t="str">
-        <v>1030513126</v>
+        <v>1030513101</v>
       </c>
       <c r="D23" t="str">
-        <v>沈苏明</v>
+        <v>陈梅婕</v>
       </c>
     </row>
     <row r="24">
@@ -726,492 +726,492 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>陈秀宏</v>
+        <v>赵燕</v>
       </c>
       <c r="B26" t="str">
-        <v>基于人眼虹膜识别的安防系统开发</v>
+        <v>基于情感体验的交互设计</v>
       </c>
       <c r="C26" t="str">
-        <v>1030513102</v>
+        <v>1030513308</v>
       </c>
       <c r="D26" t="str">
-        <v>杜亚男</v>
+        <v>梁雪晴</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>孟磊</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B27" t="str">
-        <v>面向文化场馆的分布式互动展示系统开发</v>
+        <v>无锡地区非遗的数字化保护与传承（殷俊）</v>
       </c>
       <c r="C27" t="str">
-        <v>1030513228</v>
+        <v>1030513210</v>
       </c>
       <c r="D27" t="str">
-        <v>谢尚逊</v>
+        <v>田馨月</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>孟磊</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B28" t="str">
-        <v>后工业语境下的数字技术与文化遗产整合应用方法探析</v>
+        <v>医学教学视频中的3D转制应用与设计</v>
       </c>
       <c r="C28" t="str">
-        <v>1030513202</v>
+        <v>1030513106</v>
       </c>
       <c r="D28" t="str">
-        <v>杜倩倩</v>
+        <v>贺东莉</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>丁彦蕊</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B29" t="str">
-        <v>大数据环境下的数据安全问题分析</v>
+        <v>中国大陆新闻传播学学术文献数据库建设</v>
       </c>
       <c r="C29" t="str">
-        <v>1030513318</v>
+        <v>1030513322</v>
       </c>
       <c r="D29" t="str">
-        <v>叶帼菁</v>
+        <v>郭晟</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>陈丽芳</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B30" t="str">
-        <v>基于压缩编码的数据隐藏算法的研究与实现</v>
+        <v>非遗语境下的博物馆交互性展示设计</v>
       </c>
       <c r="C30" t="str">
-        <v>1030513407</v>
+        <v>1030513206</v>
       </c>
       <c r="D30" t="str">
-        <v>洪嘉惠</v>
+        <v>刘楠</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>林意</v>
+        <v>狄岚</v>
       </c>
       <c r="B31" t="str">
-        <v>基于Unity3D屏幕特效实现</v>
+        <v>基于Unity的三维场景的交互设计与实现</v>
       </c>
       <c r="C31" t="str">
-        <v>1030513412</v>
+        <v>1030513209</v>
       </c>
       <c r="D31" t="str">
-        <v>李诗芸</v>
+        <v>马莎莎</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>林意</v>
+        <v>张军</v>
       </c>
       <c r="B32" t="str">
-        <v>OpenCV仿射变换与SURF特征点描述</v>
+        <v>基于真实云景照片的天空盒子纹理合成组件开发</v>
       </c>
       <c r="C32" t="str">
-        <v>1030513223</v>
+        <v>1030513133</v>
       </c>
       <c r="D32" t="str">
-        <v>李振明</v>
+        <v>庄蒙周</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>狄岚</v>
+        <v>晏涛</v>
       </c>
       <c r="B33" t="str">
-        <v>基于Unity的三维场景的交互设计与实现</v>
+        <v>立体图像增强和自动编辑技术研究</v>
       </c>
       <c r="C33" t="str">
-        <v>1030513209</v>
+        <v>1030513324</v>
       </c>
       <c r="D33" t="str">
-        <v>马莎莎</v>
+        <v>邱志强</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>孟磊</v>
+        <v>张军</v>
       </c>
       <c r="B34" t="str">
-        <v>基于移动互联模式改进非遗馆展项的系统开发与应用</v>
+        <v>基于DirectX的全局光照算法SVO的框架软件开发</v>
       </c>
       <c r="C34" t="str">
-        <v>1030513306</v>
+        <v>1030513408</v>
       </c>
       <c r="D34" t="str">
-        <v>李佳慧</v>
+        <v>华清沁</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>孟磊</v>
+        <v>赵燕</v>
       </c>
       <c r="B35" t="str">
-        <v>服务设计思维下非遗馆数字化展项体验优化路径研究</v>
+        <v>基于VR技术的交互设计</v>
       </c>
       <c r="C35" t="str">
-        <v>1030513216</v>
+        <v>1030513316</v>
       </c>
       <c r="D35" t="str">
-        <v>张倩倩</v>
+        <v>王君临</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>律睿敏</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B36" t="str">
-        <v>基于“六合棋”规则的解密类游戏开发</v>
+        <v>基于虚拟现实技术的地方非遗保护程序设计</v>
       </c>
       <c r="C36" t="str">
-        <v>1030513422</v>
+        <v>1030513220</v>
       </c>
       <c r="D36" t="str">
-        <v>白小山</v>
+        <v>朱雨婷</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>邓赵红</v>
+        <v>孟磊</v>
       </c>
       <c r="B37" t="str">
-        <v>网络在线人类特征识别软件开发</v>
+        <v>服务设计思维下非遗馆数字化展项体验优化路径研究</v>
       </c>
       <c r="C37" t="str">
-        <v>1030513207</v>
+        <v>1030513216</v>
       </c>
       <c r="D37" t="str">
-        <v>刘思燚</v>
+        <v>张倩倩</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>陈飞</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B38" t="str">
-        <v>cocos2d移动游戏开发</v>
+        <v>基于VR技术的校园/景区漫游</v>
       </c>
       <c r="C38" t="str">
-        <v>1030513107</v>
+        <v>1030513401</v>
       </c>
       <c r="D38" t="str">
-        <v>黄敏园</v>
+        <v>蔡青</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>陈伟</v>
+        <v>孟磊</v>
       </c>
       <c r="B39" t="str">
-        <v>魔方拼图</v>
+        <v>面向文化场馆的分布式互动展示系统开发</v>
       </c>
       <c r="C39" t="str">
-        <v>1030513125</v>
+        <v>1030513228</v>
       </c>
       <c r="D39" t="str">
-        <v>刘俊</v>
+        <v>谢尚逊</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>邓赵红</v>
+        <v>林意</v>
       </c>
       <c r="B40" t="str">
-        <v>移动端的益智游戏开发</v>
+        <v>基于Unity3D屏幕特效实现</v>
       </c>
       <c r="C40" t="str">
-        <v>1030513201</v>
+        <v>1030513412</v>
       </c>
       <c r="D40" t="str">
-        <v>陈婷婷</v>
+        <v>李诗芸</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>陈伟</v>
+        <v>邓赵红</v>
       </c>
       <c r="B41" t="str">
-        <v>像素的颜色：从算法到艺术</v>
+        <v>通用深度学习智能系统</v>
       </c>
       <c r="C41" t="str">
-        <v>1030513317</v>
+        <v>1030513130</v>
       </c>
       <c r="D41" t="str">
-        <v>杨悦</v>
+        <v>许鹏</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>王士同</v>
+        <v>陈伟</v>
       </c>
       <c r="B42" t="str">
-        <v>基于模糊聚类的图像分割及其实现</v>
+        <v>从无序到有序：点列迭代中的神奇</v>
       </c>
       <c r="C42" t="str">
-        <v>1030513421</v>
+        <v>1030513403</v>
       </c>
       <c r="D42" t="str">
-        <v>余梦巧</v>
+        <v>陈亚楠</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>邓赵红</v>
+        <v>王士同</v>
       </c>
       <c r="B43" t="str">
-        <v>通用深度学习智能系统</v>
+        <v>基于模糊聚类的图像分割及其实现</v>
       </c>
       <c r="C43" t="str">
-        <v>1030513130</v>
+        <v>1030513421</v>
       </c>
       <c r="D43" t="str">
-        <v>许鹏</v>
+        <v>余梦巧</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>张军</v>
+        <v>狄岚</v>
       </c>
       <c r="B44" t="str">
-        <v>无锡产业发展和人口成长趋势可视化调研</v>
+        <v>基于MATLAB的图像处理应用系统设计与实现</v>
       </c>
       <c r="C44" t="str">
-        <v>1030513409</v>
+        <v>1030513211</v>
       </c>
       <c r="D44" t="str">
-        <v>黄心雨</v>
+        <v>魏伊雪</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>赵燕</v>
+        <v>钱鹏江</v>
       </c>
       <c r="B45" t="str">
-        <v>三维动画设计</v>
+        <v>跨域知识学习技术及其在医学成像处理中的应用</v>
       </c>
       <c r="C45" t="str">
-        <v>1030513331</v>
+        <v>1030513320</v>
       </c>
       <c r="D45" t="str">
-        <v>吴若宇</v>
+        <v>郑佳敏</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>蒋亦樟</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B46" t="str">
-        <v>面向医学图像的图像融合技术研究</v>
+        <v>大数据环境下的数据安全问题分析</v>
       </c>
       <c r="C46" t="str">
-        <v>1030513315</v>
+        <v>1030513318</v>
       </c>
       <c r="D46" t="str">
-        <v>汤希文</v>
+        <v>叶帼菁</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>吴锋</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B47" t="str">
-        <v>境外反华群体性事件舆情监测及可视化研究（可小组执行）</v>
+        <v>基于微信的手游攻略平台设计</v>
       </c>
       <c r="C47" t="str">
-        <v>1030513127</v>
+        <v>1030513204</v>
       </c>
       <c r="D47" t="str">
-        <v>史忠源</v>
+        <v>李韵芝</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>丁彦蕊</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B48" t="str">
-        <v>基于Unity3D的VR项目设计与实现</v>
+        <v>面向甲状腺癌诊断的智能识别技术探索</v>
       </c>
       <c r="C48" t="str">
-        <v>1030513413</v>
+        <v>1030513415</v>
       </c>
       <c r="D48" t="str">
-        <v>李越敏</v>
+        <v>刘英姿</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>蒋亦樟</v>
+        <v>谢振平</v>
       </c>
       <c r="B49" t="str">
-        <v>员工任务管理系统的设计与实现</v>
+        <v>基于监控视频的会展人流特征分析及可视化</v>
       </c>
       <c r="C49" t="str">
-        <v>1030513104</v>
+        <v>1030513429</v>
       </c>
       <c r="D49" t="str">
-        <v>郭苹苹</v>
+        <v>王伟林</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>吴锋</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B50" t="str">
-        <v>中国大陆突发群体性事件数据库建设</v>
+        <v>基于matlab的气象台数据采集系统的设计与实现</v>
       </c>
       <c r="C50" t="str">
-        <v>1030513215</v>
+        <v>1030513404</v>
       </c>
       <c r="D50" t="str">
-        <v>湛倩倩</v>
+        <v>丁钰莹</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>丁彦蕊</v>
+        <v>律睿敏</v>
       </c>
       <c r="B51" t="str">
-        <v>基于matlab的气象台数据采集系统的设计与实现</v>
+        <v>一种新棋类游戏的故事化表现</v>
       </c>
       <c r="C51" t="str">
-        <v>1030513404</v>
+        <v>1030513424</v>
       </c>
       <c r="D51" t="str">
-        <v>丁钰莹</v>
+        <v>董天枢</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>陈秀宏</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B52" t="str">
-        <v>基于AR技术的手机游戏设计与开发</v>
+        <v>基于Matlab的语音信号的采集与分析</v>
       </c>
       <c r="C52" t="str">
-        <v>1030513426</v>
+        <v>1030513118</v>
       </c>
       <c r="D52" t="str">
-        <v>蒋子才</v>
+        <v>薛丹彤</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>律睿敏</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B53" t="str">
-        <v>一种新棋类游戏的故事化表现</v>
+        <v>基于AR技术的手机游戏设计与开发</v>
       </c>
       <c r="C53" t="str">
-        <v>1030513424</v>
+        <v>1030513426</v>
       </c>
       <c r="D53" t="str">
-        <v>董天枢</v>
+        <v>蒋子才</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>赵燕</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B54" t="str">
-        <v>基于Arduino的三维动画动态投影</v>
+        <v>基于人眼虹膜识别的安防系统开发</v>
       </c>
       <c r="C54" t="str">
-        <v>1030513333</v>
+        <v>1030513102</v>
       </c>
       <c r="D54" t="str">
-        <v>余帆</v>
+        <v>杜亚男</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>晏涛</v>
+        <v>张得天</v>
       </c>
       <c r="B55" t="str">
-        <v>基于图像的船型识别方法研究</v>
+        <v>Web前端开发</v>
       </c>
       <c r="C55" t="str">
-        <v>1030513414</v>
+        <v>1030513103</v>
       </c>
       <c r="D55" t="str">
-        <v>林瑞</v>
+        <v>甘姣姣</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>吴锋</v>
+        <v>邓赵红</v>
       </c>
       <c r="B56" t="str">
-        <v>“中国制造”在国外媒体的呈现框架及数据可视化分析</v>
+        <v>安卓平台人类特征识别软件开发</v>
       </c>
       <c r="C56" t="str">
-        <v>1030513110</v>
+        <v>1030513111</v>
       </c>
       <c r="D56" t="str">
-        <v>刘逸虹</v>
+        <v>龙仕清</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>陈秀宏</v>
+        <v>狄岚</v>
       </c>
       <c r="B57" t="str">
-        <v>基于AR技术的某产品宣传</v>
+        <v>基于MATLAB的人脸识别算法研究与实现</v>
       </c>
       <c r="C57" t="str">
-        <v>1030513309</v>
+        <v>1030513108</v>
       </c>
       <c r="D57" t="str">
-        <v>刘茜蓉</v>
+        <v>李贝贝</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>陈秀宏</v>
+        <v>邓赵红</v>
       </c>
       <c r="B58" t="str">
-        <v>基于VR技术的校园/景区漫游</v>
+        <v>网络在线人类特征识别软件开发</v>
       </c>
       <c r="C58" t="str">
-        <v>1030513401</v>
+        <v>1030513207</v>
       </c>
       <c r="D58" t="str">
-        <v>蔡青</v>
+        <v>刘思燚</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>谢振平</v>
+        <v>陈伟</v>
       </c>
       <c r="B59" t="str">
-        <v>大规模网络关系图的可视化研究</v>
+        <v>像素的颜色：从算法到艺术</v>
       </c>
       <c r="C59" t="str">
-        <v>1030513303</v>
+        <v>1030513317</v>
       </c>
       <c r="D59" t="str">
-        <v>陈晓琪</v>
+        <v>杨悦</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>丁彦蕊</v>
+        <v>林意</v>
       </c>
       <c r="B60" t="str">
-        <v>基于Matlab的语音信号的采集与分析</v>
+        <v>单色透明shader&amp;标准镜面高光shader</v>
       </c>
       <c r="C60" t="str">
-        <v>1030513118</v>
+        <v>1030513313</v>
       </c>
       <c r="D60" t="str">
-        <v>薛丹彤</v>
+        <v>倪晓琪</v>
       </c>
     </row>
     <row r="61">
@@ -1219,13 +1219,13 @@
         <v>陈丽芳</v>
       </c>
       <c r="B61" t="str">
-        <v>交互展陈（与艺术系老师合作）</v>
+        <v>基于压缩编码的数据隐藏算法的研究与实现</v>
       </c>
       <c r="C61" t="str">
-        <v>1030513131</v>
+        <v>1030513407</v>
       </c>
       <c r="D61" t="str">
-        <v>姚铭</v>
+        <v>洪嘉惠</v>
       </c>
     </row>
     <row r="62">
@@ -1244,58 +1244,58 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>林意</v>
+        <v>陈丽芳</v>
       </c>
       <c r="B63" t="str">
-        <v>单色透明shader&amp;标准镜面高光shader</v>
+        <v>基于视频的目标计数与目标大小计算算法研究与实现</v>
       </c>
       <c r="C63" t="str">
-        <v>1030513313</v>
+        <v>1030513304</v>
       </c>
       <c r="D63" t="str">
-        <v>倪晓琪</v>
+        <v>贺怡</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>钱鹏江</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B64" t="str">
-        <v>跨域知识学习技术及其在医学成像处理中的应用</v>
+        <v>小区物业管理系统的设计与实现</v>
       </c>
       <c r="C64" t="str">
-        <v>1030513320</v>
+        <v>1030513218</v>
       </c>
       <c r="D64" t="str">
-        <v>郑佳敏</v>
+        <v>朱静</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>钱鹏江</v>
+        <v>刘渊</v>
       </c>
       <c r="B65" t="str">
-        <v>本科毕业设计管理系统设计与实现</v>
+        <v>基于视频信息的测量与计算技术的研究</v>
       </c>
       <c r="C65" t="str">
-        <v>1030513425</v>
+        <v>1030513233</v>
       </c>
       <c r="D65" t="str">
-        <v>郭震方</v>
+        <v>郑雨杰</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>邓赵红</v>
+        <v>陈飞</v>
       </c>
       <c r="B66" t="str">
-        <v>智能图像处理软件</v>
+        <v>cocos2d移动游戏开发</v>
       </c>
       <c r="C66" t="str">
-        <v>1030513431</v>
+        <v>1030513107</v>
       </c>
       <c r="D66" t="str">
-        <v>许嘉文</v>
+        <v>黄敏园</v>
       </c>
     </row>
     <row r="67">
@@ -1314,170 +1314,170 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>赵燕</v>
+        <v>刘渊</v>
       </c>
       <c r="B68" t="str">
-        <v>基于情感体验的交互设计</v>
+        <v>社交网络的可视化研究的开发</v>
       </c>
       <c r="C68" t="str">
-        <v>1030513308</v>
+        <v>1030513310</v>
       </c>
       <c r="D68" t="str">
-        <v>梁雪晴</v>
+        <v>马驰</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>夏鸿斌</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B69" t="str">
-        <v>基于开源架构的微博情感倾向性分析</v>
+        <v>3D虚拟文物展示</v>
       </c>
       <c r="C69" t="str">
-        <v>1030513121</v>
+        <v>1030513217</v>
       </c>
       <c r="D69" t="str">
-        <v>陈衍瑜</v>
+        <v>张筱雨</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>陈伟</v>
+        <v>邓赵红</v>
       </c>
       <c r="B70" t="str">
-        <v>从无序到有序：点列迭代中的神奇</v>
+        <v>移动端的益智游戏开发</v>
       </c>
       <c r="C70" t="str">
-        <v>1030513403</v>
+        <v>1030513201</v>
       </c>
       <c r="D70" t="str">
-        <v>陈亚楠</v>
+        <v>陈婷婷</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>刘渊</v>
+        <v>狄岚</v>
       </c>
       <c r="B71" t="str">
-        <v>社交网络的可视化研究的开发</v>
+        <v>面向中学生的化学实验体验设计与实现</v>
       </c>
       <c r="C71" t="str">
-        <v>1030513310</v>
+        <v>1030513113</v>
       </c>
       <c r="D71" t="str">
-        <v>马驰</v>
+        <v>欧嘉琳</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>夏鸿斌</v>
+        <v>邓赵红</v>
       </c>
       <c r="B72" t="str">
-        <v>基于LEAP Motion的手势识别技术构建新闻头条浏览系统</v>
+        <v>智能图像处理软件</v>
       </c>
       <c r="C72" t="str">
-        <v>1030513410</v>
+        <v>1030513431</v>
       </c>
       <c r="D72" t="str">
-        <v>贾玉珍</v>
+        <v>许嘉文</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>陈秀宏</v>
+        <v>孟磊</v>
       </c>
       <c r="B73" t="str">
-        <v>3D虚拟文物展示</v>
+        <v>基于移动互联模式改进非遗馆展项的系统开发与应用</v>
       </c>
       <c r="C73" t="str">
-        <v>1030513217</v>
+        <v>1030513306</v>
       </c>
       <c r="D73" t="str">
-        <v>张筱雨</v>
+        <v>李佳慧</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>丁彦蕊</v>
+        <v>张得天</v>
       </c>
       <c r="B74" t="str">
-        <v>基于3ds max的城市小区动画漫游设计与实现</v>
+        <v>微信公众号前端开发</v>
       </c>
       <c r="C74" t="str">
-        <v>1030513119</v>
+        <v>1030513112</v>
       </c>
       <c r="D74" t="str">
-        <v>姚陆吉</v>
+        <v>毛姝婧</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>丁彦蕊</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B75" t="str">
-        <v>基于微信的手游攻略平台设计</v>
+        <v>面向医学图像的图像融合技术研究</v>
       </c>
       <c r="C75" t="str">
-        <v>1030513204</v>
+        <v>1030513315</v>
       </c>
       <c r="D75" t="str">
-        <v>李韵芝</v>
+        <v>汤希文</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>陈丽芳</v>
+        <v>张得天</v>
       </c>
       <c r="B76" t="str">
-        <v>基于视频的目标计数与目标大小计算算法研究与实现</v>
+        <v>基于企业数据的爬虫</v>
       </c>
       <c r="C76" t="str">
-        <v>1030513304</v>
+        <v>1030513129</v>
       </c>
       <c r="D76" t="str">
-        <v>贺怡</v>
+        <v>王斌</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>钱鹏江</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B77" t="str">
-        <v>MapReduce分布式计算架构分析与实践</v>
+        <v>基于智能方法的癫痫脑电信号识别研究</v>
       </c>
       <c r="C77" t="str">
-        <v>1030513420</v>
+        <v>1030513208</v>
       </c>
       <c r="D77" t="str">
-        <v>杨艺</v>
+        <v>卢虹羽</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>黄秋儒</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B78" t="str">
-        <v>医学教学视频中的3D转制应用与设计</v>
+        <v>旅行社信息管理系统的设计与实现</v>
       </c>
       <c r="C78" t="str">
-        <v>1030513106</v>
+        <v>1030513205</v>
       </c>
       <c r="D78" t="str">
-        <v>贺东莉</v>
+        <v>刘孟楠</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>陈丽芳</v>
+        <v>谢振平</v>
       </c>
       <c r="B79" t="str">
-        <v>基于视频的目标识别与标记系统的研究与实现</v>
+        <v>大规模网络关系图的可视化研究</v>
       </c>
       <c r="C79" t="str">
-        <v>1030513203</v>
+        <v>1030513303</v>
       </c>
       <c r="D79" t="str">
-        <v>李明泉</v>
+        <v>陈晓琪</v>
       </c>
     </row>
     <row r="80">
@@ -1496,324 +1496,254 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>律睿敏</v>
+        <v>林意</v>
       </c>
       <c r="B81" t="str">
-        <v>具有音频编辑与分享功能的音乐播放器开发</v>
+        <v>OpenCV仿射变换与SURF特征点描述</v>
       </c>
       <c r="C81" t="str">
-        <v>1030513232</v>
+        <v>1030513223</v>
       </c>
       <c r="D81" t="str">
-        <v>杨笑寒</v>
+        <v>李振明</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>律睿敏</v>
+        <v>林意</v>
       </c>
       <c r="B82" t="str">
-        <v>“六合棋”的人机对战AI算法设计</v>
+        <v>OpenCV边缘检测之比较</v>
       </c>
       <c r="C82" t="str">
-        <v>1030513222</v>
+        <v>1030513124</v>
       </c>
       <c r="D82" t="str">
-        <v>李嘉文</v>
+        <v>刘家旺</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>吴锋</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B83" t="str">
-        <v>亚投行的国际舆情监测及数据可视化分析</v>
+        <v>基于3ds max的城市小区动画漫游设计与实现</v>
       </c>
       <c r="C83" t="str">
-        <v>1030513109</v>
+        <v>1030513119</v>
       </c>
       <c r="D83" t="str">
-        <v>李丹</v>
+        <v>姚陆吉</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>陈秀宏</v>
+        <v>张军</v>
       </c>
       <c r="B84" t="str">
-        <v>视频目标跟踪方法研究与实现</v>
+        <v>无锡产业发展和人口成长趋势可视化调研</v>
       </c>
       <c r="C84" t="str">
-        <v>1030512302</v>
+        <v>1030513409</v>
       </c>
       <c r="D84" t="str">
-        <v>方旭</v>
+        <v>黄心雨</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>陈秀宏</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B85" t="str">
-        <v>图像特征与识别方法的研究与实现</v>
+        <v>基于开源架构的微博情感倾向性分析</v>
       </c>
       <c r="C85" t="str">
-        <v>1030513128</v>
+        <v>1030513121</v>
       </c>
       <c r="D85" t="str">
-        <v>孙锐</v>
+        <v>陈衍瑜</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>林意</v>
+        <v>陈飞</v>
       </c>
       <c r="B86" t="str">
-        <v>OpenCV边缘检测之比较</v>
+        <v>基于construct2的HTML5游戏开发</v>
       </c>
       <c r="C86" t="str">
-        <v>1030513124</v>
+        <v>1030513120</v>
       </c>
       <c r="D86" t="str">
-        <v>刘家旺</v>
+        <v>于思涵</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>黄秋儒</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B87" t="str">
-        <v>中国大陆新闻传播学学术文献数据库建设</v>
+        <v>基于LEAP Motion的手势识别技术构建新闻头条浏览系统</v>
       </c>
       <c r="C87" t="str">
-        <v>1030513322</v>
+        <v>1030513410</v>
       </c>
       <c r="D87" t="str">
-        <v>郭晟</v>
+        <v>贾玉珍</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>狄岚</v>
+        <v>晏涛</v>
       </c>
       <c r="B88" t="str">
-        <v>基于MATLAB的人脸识别算法研究与实现</v>
+        <v>立体图像匹配技术研究</v>
       </c>
       <c r="C88" t="str">
-        <v>1030513108</v>
+        <v>1030513326</v>
       </c>
       <c r="D88" t="str">
-        <v>李贝贝</v>
+        <v>苏德志</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>黄秋儒</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B89" t="str">
-        <v>基于虚拟现实技术的地方非遗保护程序设计</v>
+        <v>员工任务管理系统的设计与实现</v>
       </c>
       <c r="C89" t="str">
-        <v>1030513220</v>
+        <v>1030513104</v>
       </c>
       <c r="D89" t="str">
-        <v>朱雨婷</v>
+        <v>郭苹苹</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>律睿敏</v>
+        <v>陈飞</v>
       </c>
       <c r="B90" t="str">
-        <v>绘画解密游戏设计</v>
+        <v>基于Jquery的Web前端应用开发</v>
       </c>
       <c r="C90" t="str">
-        <v>1030513122</v>
+        <v>1030513132</v>
       </c>
       <c r="D90" t="str">
-        <v>金振阳</v>
+        <v>张俊操</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>黄秋儒</v>
+        <v>赵燕</v>
       </c>
       <c r="B91" t="str">
-        <v>非遗语境下的博物馆交互性展示设计</v>
+        <v>基于Arduino的三维动画动态投影</v>
       </c>
       <c r="C91" t="str">
-        <v>1030513206</v>
+        <v>1030513333</v>
       </c>
       <c r="D91" t="str">
-        <v>刘楠</v>
+        <v>余帆</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>狄岚</v>
+        <v>陈飞</v>
       </c>
       <c r="B92" t="str">
-        <v>面向中学生的化学实验体验设计与实现</v>
+        <v>微信小程序开发</v>
       </c>
       <c r="C92" t="str">
-        <v>1030513113</v>
+        <v>1030513231</v>
       </c>
       <c r="D92" t="str">
-        <v>欧嘉琳</v>
+        <v>许军</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>张得天</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B93" t="str">
-        <v>微信公众号前端开发</v>
+        <v>基于视频特效的影视短片制作</v>
       </c>
       <c r="C93" t="str">
-        <v>1030513112</v>
+        <v>1030513311</v>
       </c>
       <c r="D93" t="str">
-        <v>毛姝婧</v>
+        <v>马鲁昕</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>黄秋儒</v>
+        <v>陈丽芳</v>
       </c>
       <c r="B94" t="str">
-        <v>基于视频特效的影视短片制作</v>
+        <v>基于视频的目标识别与标记系统的研究与实现</v>
       </c>
       <c r="C94" t="str">
-        <v>1030513311</v>
+        <v>1030513203</v>
       </c>
       <c r="D94" t="str">
-        <v>马鲁昕</v>
+        <v>李明泉</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>黄秋儒</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B95" t="str">
-        <v>无锡地区非遗的数字化保护与传承（殷俊）</v>
+        <v>图像特征与识别方法的研究与实现</v>
       </c>
       <c r="C95" t="str">
-        <v>1030513210</v>
+        <v>1030513128</v>
       </c>
       <c r="D95" t="str">
-        <v>田馨月</v>
+        <v>孙锐</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>狄岚</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B96" t="str">
-        <v>基于MATLAB的图像处理应用系统设计与实现</v>
+        <v>基于Unity3D的VR项目设计与实现</v>
       </c>
       <c r="C96" t="str">
-        <v>1030513211</v>
+        <v>1030513413</v>
       </c>
       <c r="D96" t="str">
-        <v>魏伊雪</v>
+        <v>李越敏</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>陈飞</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B97" t="str">
-        <v>基于construct2的HTML5游戏开发</v>
+        <v>基于AR技术的某产品宣传</v>
       </c>
       <c r="C97" t="str">
-        <v>1030513120</v>
+        <v>1030513309</v>
       </c>
       <c r="D97" t="str">
-        <v>于思涵</v>
+        <v>刘茜蓉</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>晏涛</v>
+        <v>陈丽芳</v>
       </c>
       <c r="B98" t="str">
-        <v>立体图像匹配技术研究</v>
+        <v>交互展陈（与艺术系老师合作）</v>
       </c>
       <c r="C98" t="str">
-        <v>1030513326</v>
+        <v>1030513131</v>
       </c>
       <c r="D98" t="str">
-        <v>苏德志</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="str">
-        <v>晏涛</v>
-      </c>
-      <c r="B99" t="str">
-        <v>立体图像增强和自动编辑技术研究</v>
-      </c>
-      <c r="C99" t="str">
-        <v>1030513324</v>
-      </c>
-      <c r="D99" t="str">
-        <v>邱志强</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="str">
-        <v>陈飞</v>
-      </c>
-      <c r="B100" t="str">
-        <v>基于Jquery的Web前端应用开发</v>
-      </c>
-      <c r="C100" t="str">
-        <v>1030513132</v>
-      </c>
-      <c r="D100" t="str">
-        <v>张俊操</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="str">
-        <v>夏鸿斌</v>
-      </c>
-      <c r="B101" t="str">
-        <v>基于用户行为的电影推荐系统构建</v>
-      </c>
-      <c r="C101" t="str">
-        <v>1030513213</v>
-      </c>
-      <c r="D101" t="str">
-        <v>徐慧敏</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="str">
-        <v>晏涛</v>
-      </c>
-      <c r="B102" t="str">
-        <v>多视点图像新视点生成技术研究</v>
-      </c>
-      <c r="C102" t="str">
-        <v>1030513328</v>
-      </c>
-      <c r="D102" t="str">
-        <v>王家麟</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="str">
-        <v>张得天</v>
-      </c>
-      <c r="B103" t="str">
-        <v>Web前端开发</v>
-      </c>
-      <c r="C103" t="str">
-        <v>1030513103</v>
-      </c>
-      <c r="D103" t="str">
-        <v>甘姣姣</v>
+        <v>姚铭</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backup before update interface
</commit_message>
<xml_diff>
--- a/server/files/download/SelectedResult.xlsx
+++ b/server/files/download/SelectedResult.xlsx
@@ -390,296 +390,296 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>夏鸿斌</v>
+        <v>赵燕</v>
       </c>
       <c r="B2" t="str">
-        <v>基于开源架构的微博情感倾向性分析</v>
+        <v>基于VR技术的交互设计</v>
       </c>
       <c r="C2" t="str">
-        <v>1030513121</v>
+        <v>1030513316</v>
       </c>
       <c r="D2" t="str">
-        <v>陈衍瑜</v>
+        <v>王君临</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>陈飞</v>
+        <v>张军</v>
       </c>
       <c r="B3" t="str">
-        <v>微信小程序开发</v>
+        <v>无锡产业发展和人口成长趋势可视化调研</v>
       </c>
       <c r="C3" t="str">
-        <v>1030513231</v>
+        <v>1030513409</v>
       </c>
       <c r="D3" t="str">
-        <v>许军</v>
+        <v>黄心雨</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>夏鸿斌</v>
+        <v>狄岚</v>
       </c>
       <c r="B4" t="str">
-        <v>基于用户行为的电影推荐系统构建</v>
+        <v>图像分割算法的研究与实现</v>
       </c>
       <c r="C4" t="str">
-        <v>1030513213</v>
+        <v>1030513305</v>
       </c>
       <c r="D4" t="str">
-        <v>徐慧敏</v>
+        <v>矫慧文</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>陈飞</v>
+        <v>赵燕</v>
       </c>
       <c r="B5" t="str">
-        <v>基于ffmpeg的视频应用开发</v>
+        <v>三维动画设计</v>
       </c>
       <c r="C5" t="str">
-        <v>1030513126</v>
+        <v>1030513331</v>
       </c>
       <c r="D5" t="str">
-        <v>沈苏明</v>
+        <v>吴若宇</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>陈伟</v>
+        <v>张军</v>
       </c>
       <c r="B6" t="str">
-        <v>像素的颜色：从算法到艺术</v>
+        <v>基于真实云景照片的天空盒子纹理合成组件开发</v>
       </c>
       <c r="C6" t="str">
-        <v>1030513317</v>
+        <v>1030513133</v>
       </c>
       <c r="D6" t="str">
-        <v>杨悦</v>
+        <v>庄蒙周</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>赵燕</v>
+        <v>狄岚</v>
       </c>
       <c r="B7" t="str">
-        <v>基于Arduino的三维动画动态投影</v>
+        <v>基于MATLAB的人脸识别算法研究与实现</v>
       </c>
       <c r="C7" t="str">
-        <v>1030513333</v>
+        <v>1030513108</v>
       </c>
       <c r="D7" t="str">
-        <v>余帆</v>
+        <v>李贝贝</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>王士同</v>
+        <v>赵燕</v>
       </c>
       <c r="B8" t="str">
-        <v>基于模糊聚类的图像分割及其实现</v>
+        <v>绘本的动态化数字展示</v>
       </c>
       <c r="C8" t="str">
-        <v>1030513421</v>
+        <v>1030513423</v>
       </c>
       <c r="D8" t="str">
-        <v>余梦巧</v>
+        <v>曹钰</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>狄岚</v>
+        <v>王士同</v>
       </c>
       <c r="B9" t="str">
-        <v>基于MATLAB的人脸识别算法研究与实现</v>
+        <v>基于模糊聚类的图像分割及其实现</v>
       </c>
       <c r="C9" t="str">
-        <v>1030513108</v>
+        <v>1030513421</v>
       </c>
       <c r="D9" t="str">
-        <v>李贝贝</v>
+        <v>余梦巧</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>赵燕</v>
+        <v>狄岚</v>
       </c>
       <c r="B10" t="str">
-        <v>AR技术在购物环境应用下的交互设计</v>
+        <v>基于Unity的三维场景的交互设计与实现</v>
       </c>
       <c r="C10" t="str">
-        <v>1030513416</v>
+        <v>1030513209</v>
       </c>
       <c r="D10" t="str">
-        <v>彭开云</v>
+        <v>马莎莎</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>夏鸿斌</v>
+        <v>赵燕</v>
       </c>
       <c r="B11" t="str">
-        <v>基于html5的移动应用开发</v>
+        <v>AR技术在购物环境应用下的交互设计</v>
       </c>
       <c r="C11" t="str">
-        <v>1030513319</v>
+        <v>1030513416</v>
       </c>
       <c r="D11" t="str">
-        <v>赵欢</v>
+        <v>彭开云</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>刘渊</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B12" t="str">
-        <v>基于视频信息的测量与计算技术的研究</v>
+        <v>基于html5的移动应用开发</v>
       </c>
       <c r="C12" t="str">
-        <v>1030513233</v>
+        <v>1030513319</v>
       </c>
       <c r="D12" t="str">
-        <v>郑雨杰</v>
+        <v>赵欢</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>赵燕</v>
+        <v>刘渊</v>
       </c>
       <c r="B13" t="str">
-        <v>基于VR技术的交互设计</v>
+        <v>社交网络的可视化研究的开发</v>
       </c>
       <c r="C13" t="str">
-        <v>1030513316</v>
+        <v>1030513310</v>
       </c>
       <c r="D13" t="str">
-        <v>王君临</v>
+        <v>马驰</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>张军</v>
+        <v>赵燕</v>
       </c>
       <c r="B14" t="str">
-        <v>无锡产业发展和人口成长趋势可视化调研</v>
+        <v>基于情感体验的交互设计</v>
       </c>
       <c r="C14" t="str">
-        <v>1030513409</v>
+        <v>1030513308</v>
       </c>
       <c r="D14" t="str">
-        <v>黄心雨</v>
+        <v>梁雪晴</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>狄岚</v>
+        <v>陈飞</v>
       </c>
       <c r="B15" t="str">
-        <v>基于Unity的三维场景的交互设计与实现</v>
+        <v>cocos2d移动游戏开发</v>
       </c>
       <c r="C15" t="str">
-        <v>1030513209</v>
+        <v>1030513107</v>
       </c>
       <c r="D15" t="str">
-        <v>马莎莎</v>
+        <v>黄敏园</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>张军</v>
+        <v>狄岚</v>
       </c>
       <c r="B16" t="str">
-        <v>基于真实云景照片的天空盒子纹理合成组件开发</v>
+        <v>面向中学生的化学实验体验设计与实现</v>
       </c>
       <c r="C16" t="str">
-        <v>1030513133</v>
+        <v>1030513113</v>
       </c>
       <c r="D16" t="str">
-        <v>庄蒙周</v>
+        <v>欧嘉琳</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>陈飞</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B17" t="str">
-        <v>基于Jquery的Web前端应用开发</v>
+        <v>基于开源架构的微博情感倾向性分析</v>
       </c>
       <c r="C17" t="str">
-        <v>1030513132</v>
+        <v>1030513121</v>
       </c>
       <c r="D17" t="str">
-        <v>张俊操</v>
+        <v>陈衍瑜</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>陈伟</v>
+        <v>陈飞</v>
       </c>
       <c r="B18" t="str">
-        <v>魔方拼图</v>
+        <v>基于ffmpeg的视频应用开发</v>
       </c>
       <c r="C18" t="str">
-        <v>1030513125</v>
+        <v>1030513126</v>
       </c>
       <c r="D18" t="str">
-        <v>刘俊</v>
+        <v>沈苏明</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>夏鸿斌</v>
+        <v>陈伟</v>
       </c>
       <c r="B19" t="str">
-        <v>与艺术性合作：基于unity交互引擎的数字艺术表现(章立)</v>
+        <v>从无序到有序：点列迭代中的神奇</v>
       </c>
       <c r="C19" t="str">
-        <v>1030513314</v>
+        <v>1030513403</v>
       </c>
       <c r="D19" t="str">
-        <v>史罗琼</v>
+        <v>陈亚楠</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>陈飞</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B20" t="str">
-        <v>cocos2d移动游戏开发</v>
+        <v>与艺术性合作：基于unity交互引擎的数字艺术表现(章立)</v>
       </c>
       <c r="C20" t="str">
-        <v>1030513107</v>
+        <v>1030513314</v>
       </c>
       <c r="D20" t="str">
-        <v>黄敏园</v>
+        <v>史罗琼</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>狄岚</v>
+        <v>陈飞</v>
       </c>
       <c r="B21" t="str">
-        <v>基于MATLAB的图像处理应用系统设计与实现</v>
+        <v>基于construct2的HTML5游戏开发</v>
       </c>
       <c r="C21" t="str">
-        <v>1030513211</v>
+        <v>1030513120</v>
       </c>
       <c r="D21" t="str">
-        <v>魏伊雪</v>
+        <v>于思涵</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>赵燕</v>
+        <v>狄岚</v>
       </c>
       <c r="B22" t="str">
-        <v>绘本的动态化数字展示</v>
+        <v>基于MATLAB的图像处理应用系统设计与实现</v>
       </c>
       <c r="C22" t="str">
-        <v>1030513423</v>
+        <v>1030513211</v>
       </c>
       <c r="D22" t="str">
-        <v>曹钰</v>
+        <v>魏伊雪</v>
       </c>
     </row>
     <row r="23">
@@ -698,282 +698,282 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>刘渊</v>
+        <v>陈飞</v>
       </c>
       <c r="B24" t="str">
-        <v>社交网络的可视化研究的开发</v>
+        <v>基于Jquery的Web前端应用开发</v>
       </c>
       <c r="C24" t="str">
-        <v>1030513310</v>
+        <v>1030513132</v>
       </c>
       <c r="D24" t="str">
-        <v>马驰</v>
+        <v>张俊操</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>邓赵红</v>
+        <v>赵燕</v>
       </c>
       <c r="B25" t="str">
-        <v>安卓平台人类特征识别软件开发</v>
+        <v>基于Arduino的三维动画动态投影</v>
       </c>
       <c r="C25" t="str">
-        <v>1030513111</v>
+        <v>1030513333</v>
       </c>
       <c r="D25" t="str">
-        <v>龙仕清</v>
+        <v>余帆</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>赵燕</v>
+        <v>张军</v>
       </c>
       <c r="B26" t="str">
-        <v>基于情感体验的交互设计</v>
+        <v>基于DirectX的全局光照算法SVO的框架软件开发</v>
       </c>
       <c r="C26" t="str">
-        <v>1030513308</v>
+        <v>1030513408</v>
       </c>
       <c r="D26" t="str">
-        <v>梁雪晴</v>
+        <v>华清沁</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>陈飞</v>
+        <v>刘渊</v>
       </c>
       <c r="B27" t="str">
-        <v>基于construct2的HTML5游戏开发</v>
+        <v>基于视频信息的测量与计算技术的研究</v>
       </c>
       <c r="C27" t="str">
-        <v>1030513120</v>
+        <v>1030513233</v>
       </c>
       <c r="D27" t="str">
-        <v>于思涵</v>
+        <v>郑雨杰</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>狄岚</v>
+        <v>夏鸿斌</v>
       </c>
       <c r="B28" t="str">
-        <v>面向中学生的化学实验体验设计与实现</v>
+        <v>基于用户行为的电影推荐系统构建</v>
       </c>
       <c r="C28" t="str">
-        <v>1030513113</v>
+        <v>1030513213</v>
       </c>
       <c r="D28" t="str">
-        <v>欧嘉琳</v>
+        <v>徐慧敏</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>赵燕</v>
+        <v>陈飞</v>
       </c>
       <c r="B29" t="str">
-        <v>三维动画设计</v>
+        <v>微信小程序开发</v>
       </c>
       <c r="C29" t="str">
-        <v>1030513331</v>
+        <v>1030513231</v>
       </c>
       <c r="D29" t="str">
-        <v>吴若宇</v>
+        <v>许军</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>张军</v>
+        <v>陈伟</v>
       </c>
       <c r="B30" t="str">
-        <v>基于DirectX的全局光照算法SVO的框架软件开发</v>
+        <v>像素的颜色：从算法到艺术</v>
       </c>
       <c r="C30" t="str">
-        <v>1030513408</v>
+        <v>1030513317</v>
       </c>
       <c r="D30" t="str">
-        <v>华清沁</v>
+        <v>杨悦</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>狄岚</v>
+        <v>邓赵红</v>
       </c>
       <c r="B31" t="str">
-        <v>图像分割算法的研究与实现</v>
+        <v>移动端的益智游戏开发</v>
       </c>
       <c r="C31" t="str">
-        <v>1030513305</v>
+        <v>1030513201</v>
       </c>
       <c r="D31" t="str">
-        <v>矫慧文</v>
+        <v>陈婷婷</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>陈伟</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B32" t="str">
-        <v>从无序到有序：点列迭代中的神奇</v>
+        <v>基于VR技术的校园/景区漫游</v>
       </c>
       <c r="C32" t="str">
-        <v>1030513403</v>
+        <v>1030513401</v>
       </c>
       <c r="D32" t="str">
-        <v>陈亚楠</v>
+        <v>蔡青</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>孟磊</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B33" t="str">
-        <v>服务设计思维下非遗馆数字化展项体验优化路径研究</v>
+        <v>小区物业管理系统的设计与实现</v>
       </c>
       <c r="C33" t="str">
-        <v>1030513216</v>
+        <v>1030513218</v>
       </c>
       <c r="D33" t="str">
-        <v>张倩倩</v>
+        <v>朱静</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>蒋亦樟</v>
+        <v>谢振平</v>
       </c>
       <c r="B34" t="str">
-        <v>小区物业管理系统的设计与实现</v>
+        <v>大规模网络关系图的可视化研究</v>
       </c>
       <c r="C34" t="str">
-        <v>1030513218</v>
+        <v>1030513303</v>
       </c>
       <c r="D34" t="str">
-        <v>朱静</v>
+        <v>陈晓琪</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>林意</v>
+        <v>律睿敏</v>
       </c>
       <c r="B35" t="str">
-        <v>基于Unity3D屏幕特效实现</v>
+        <v>“六合棋”的人机对战AI算法设计</v>
       </c>
       <c r="C35" t="str">
-        <v>1030513412</v>
+        <v>1030513222</v>
       </c>
       <c r="D35" t="str">
-        <v>李诗芸</v>
+        <v>李嘉文</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>陈秀宏</v>
+        <v>张得天</v>
       </c>
       <c r="B36" t="str">
-        <v>基于人眼虹膜识别的安防系统开发</v>
+        <v>垂直爬虫开发</v>
       </c>
       <c r="C36" t="str">
-        <v>1030513102</v>
+        <v>1030513332</v>
       </c>
       <c r="D36" t="str">
-        <v>杜亚男</v>
+        <v>肖山民</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>陈丽芳</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B37" t="str">
-        <v>多维信息展示的课程辅助教学系统的研究与实现</v>
+        <v>非遗语境下的博物馆交互性展示设计</v>
       </c>
       <c r="C37" t="str">
-        <v>1030513402</v>
+        <v>1030513206</v>
       </c>
       <c r="D37" t="str">
-        <v>陈慧敏</v>
+        <v>刘楠</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>林意</v>
+        <v>钱鹏江</v>
       </c>
       <c r="B38" t="str">
-        <v>OpenCV哈夫变换线圆检测实现</v>
+        <v>MapReduce分布式计算架构分析与实践</v>
       </c>
       <c r="C38" t="str">
-        <v>1030513221</v>
+        <v>1030513420</v>
       </c>
       <c r="D38" t="str">
-        <v>戴杰</v>
+        <v>杨艺</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>孟磊</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B39" t="str">
-        <v>面向文化场馆的分布式互动展示系统开发</v>
+        <v>视频目标跟踪方法研究与实现</v>
       </c>
       <c r="C39" t="str">
-        <v>1030513228</v>
+        <v>1030512302</v>
       </c>
       <c r="D39" t="str">
-        <v>谢尚逊</v>
+        <v>方旭</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>蒋亦樟</v>
+        <v>林意</v>
       </c>
       <c r="B40" t="str">
-        <v>面向医学图像的图像融合技术研究</v>
+        <v>单色透明shader&amp;标准镜面高光shader</v>
       </c>
       <c r="C40" t="str">
-        <v>1030513315</v>
+        <v>1030513313</v>
       </c>
       <c r="D40" t="str">
-        <v>汤希文</v>
+        <v>倪晓琪</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>律睿敏</v>
+        <v>晏涛</v>
       </c>
       <c r="B41" t="str">
-        <v>一种新棋类游戏的故事化表现</v>
+        <v>基于图像的船型识别方法研究</v>
       </c>
       <c r="C41" t="str">
-        <v>1030513424</v>
+        <v>1030513414</v>
       </c>
       <c r="D41" t="str">
-        <v>董天枢</v>
+        <v>林瑞</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>蒋亦樟</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B42" t="str">
-        <v>旅行社信息管理系统的设计与实现</v>
+        <v>基于matlab的气象台数据采集系统的设计与实现</v>
       </c>
       <c r="C42" t="str">
-        <v>1030513205</v>
+        <v>1030513404</v>
       </c>
       <c r="D42" t="str">
-        <v>刘孟楠</v>
+        <v>丁钰莹</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>黄秋儒</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B43" t="str">
-        <v>基于视频特效的影视短片制作</v>
+        <v>面向医学图像的图像融合技术研究</v>
       </c>
       <c r="C43" t="str">
-        <v>1030513311</v>
+        <v>1030513315</v>
       </c>
       <c r="D43" t="str">
-        <v>马鲁昕</v>
+        <v>汤希文</v>
       </c>
     </row>
     <row r="44">
@@ -981,209 +981,209 @@
         <v>黄秋儒</v>
       </c>
       <c r="B44" t="str">
-        <v>医学教学视频中的3D转制应用与设计</v>
+        <v>中国大陆新闻传播学学术文献数据库建设</v>
       </c>
       <c r="C44" t="str">
-        <v>1030513106</v>
+        <v>1030513322</v>
       </c>
       <c r="D44" t="str">
-        <v>贺东莉</v>
+        <v>郭晟</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>律睿敏</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B45" t="str">
-        <v>绘画解密游戏设计</v>
+        <v>基于视频特效的影视短片制作</v>
       </c>
       <c r="C45" t="str">
-        <v>1030513122</v>
+        <v>1030513311</v>
       </c>
       <c r="D45" t="str">
-        <v>金振阳</v>
+        <v>马鲁昕</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>钱鹏江</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B46" t="str">
-        <v>MapReduce分布式计算架构分析与实践</v>
+        <v>大数据环境下的数据安全问题分析</v>
       </c>
       <c r="C46" t="str">
-        <v>1030513420</v>
+        <v>1030513318</v>
       </c>
       <c r="D46" t="str">
-        <v>杨艺</v>
+        <v>叶帼菁</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>丁彦蕊</v>
+        <v>陈丽芳</v>
       </c>
       <c r="B47" t="str">
-        <v>基于微信的手游攻略平台设计</v>
+        <v>基于视频的目标计数与目标大小计算算法研究与实现</v>
       </c>
       <c r="C47" t="str">
-        <v>1030513204</v>
+        <v>1030513304</v>
       </c>
       <c r="D47" t="str">
-        <v>李韵芝</v>
+        <v>贺怡</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>邓赵红</v>
+        <v>律睿敏</v>
       </c>
       <c r="B48" t="str">
-        <v>移动端的益智游戏开发</v>
+        <v>具有音频编辑与分享功能的音乐播放器开发</v>
       </c>
       <c r="C48" t="str">
-        <v>1030513201</v>
+        <v>1030513232</v>
       </c>
       <c r="D48" t="str">
-        <v>陈婷婷</v>
+        <v>杨笑寒</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>丁彦蕊</v>
+        <v>孟磊</v>
       </c>
       <c r="B49" t="str">
-        <v>基于matlab的气象台数据采集系统的设计与实现</v>
+        <v>服务设计思维下非遗馆数字化展项体验优化路径研究</v>
       </c>
       <c r="C49" t="str">
-        <v>1030513404</v>
+        <v>1030513216</v>
       </c>
       <c r="D49" t="str">
-        <v>丁钰莹</v>
+        <v>张倩倩</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>晏涛</v>
+        <v>谢振平</v>
       </c>
       <c r="B50" t="str">
-        <v>基于图像的船型识别方法研究</v>
+        <v>大数据行为特征智能挖掘技术研究</v>
       </c>
       <c r="C50" t="str">
-        <v>1030513414</v>
+        <v>1030513101</v>
       </c>
       <c r="D50" t="str">
-        <v>林瑞</v>
+        <v>陈梅婕</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>晏涛</v>
+        <v>孟磊</v>
       </c>
       <c r="B51" t="str">
-        <v>本科毕业设计管理系统设计与实现</v>
+        <v>面向文化场馆的分布式互动展示系统开发</v>
       </c>
       <c r="C51" t="str">
-        <v>1030513430</v>
+        <v>1030513228</v>
       </c>
       <c r="D51" t="str">
-        <v>吴吉</v>
+        <v>谢尚逊</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>陈丽芳</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B52" t="str">
-        <v>基于压缩编码的数据隐藏算法的研究与实现</v>
+        <v>面向甲状腺癌诊断的智能识别技术探索</v>
       </c>
       <c r="C52" t="str">
-        <v>1030513407</v>
+        <v>1030513415</v>
       </c>
       <c r="D52" t="str">
-        <v>洪嘉惠</v>
+        <v>刘英姿</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>蒋亦樟</v>
+        <v>陈伟</v>
       </c>
       <c r="B53" t="str">
-        <v>基于智能方法的癫痫脑电信号识别研究</v>
+        <v>魔方拼图</v>
       </c>
       <c r="C53" t="str">
-        <v>1030513208</v>
+        <v>1030513125</v>
       </c>
       <c r="D53" t="str">
-        <v>卢虹羽</v>
+        <v>刘俊</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>钱鹏江</v>
+        <v>邓赵红</v>
       </c>
       <c r="B54" t="str">
-        <v>跨域知识学习技术及其在医学成像处理中的应用</v>
+        <v>网络在线人类特征识别软件开发</v>
       </c>
       <c r="C54" t="str">
-        <v>1030513320</v>
+        <v>1030513207</v>
       </c>
       <c r="D54" t="str">
-        <v>郑佳敏</v>
+        <v>刘思燚</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>谢振平</v>
+        <v>陈丽芳</v>
       </c>
       <c r="B55" t="str">
-        <v>大规模网络关系图的可视化研究</v>
+        <v>多维信息展示的课程辅助教学系统的研究与实现</v>
       </c>
       <c r="C55" t="str">
-        <v>1030513303</v>
+        <v>1030513402</v>
       </c>
       <c r="D55" t="str">
-        <v>陈晓琪</v>
+        <v>陈慧敏</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>黄秋儒</v>
+        <v>邓赵红</v>
       </c>
       <c r="B56" t="str">
-        <v>基于虚拟现实技术的地方非遗保护程序设计</v>
+        <v>智能图像处理软件</v>
       </c>
       <c r="C56" t="str">
-        <v>1030513220</v>
+        <v>1030513431</v>
       </c>
       <c r="D56" t="str">
-        <v>朱雨婷</v>
+        <v>许嘉文</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>张得天</v>
+        <v>林意</v>
       </c>
       <c r="B57" t="str">
-        <v>微信公众号前端开发</v>
+        <v>OpenCV哈夫变换线圆检测实现</v>
       </c>
       <c r="C57" t="str">
-        <v>1030513112</v>
+        <v>1030513221</v>
       </c>
       <c r="D57" t="str">
-        <v>毛姝婧</v>
+        <v>戴杰</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>丁彦蕊</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B58" t="str">
-        <v>基于Unity3D的VR项目设计与实现</v>
+        <v>基于AR技术的某产品宣传</v>
       </c>
       <c r="C58" t="str">
-        <v>1030513413</v>
+        <v>1030513309</v>
       </c>
       <c r="D58" t="str">
-        <v>李越敏</v>
+        <v>刘茜蓉</v>
       </c>
     </row>
     <row r="59">
@@ -1191,13 +1191,13 @@
         <v>丁彦蕊</v>
       </c>
       <c r="B59" t="str">
-        <v>基于Matlab的语音信号的采集与分析</v>
+        <v>基于3ds max的城市小区动画漫游设计与实现</v>
       </c>
       <c r="C59" t="str">
-        <v>1030513118</v>
+        <v>1030513119</v>
       </c>
       <c r="D59" t="str">
-        <v>薛丹彤</v>
+        <v>姚陆吉</v>
       </c>
     </row>
     <row r="60">
@@ -1205,41 +1205,41 @@
         <v>陈秀宏</v>
       </c>
       <c r="B60" t="str">
-        <v>基于AR技术的某产品宣传</v>
+        <v>3D虚拟文物展示</v>
       </c>
       <c r="C60" t="str">
-        <v>1030513309</v>
+        <v>1030513217</v>
       </c>
       <c r="D60" t="str">
-        <v>刘茜蓉</v>
+        <v>张筱雨</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>张得天</v>
+        <v>邓赵红</v>
       </c>
       <c r="B61" t="str">
-        <v>欺诈短信的数据挖掘</v>
+        <v>通用深度学习智能系统</v>
       </c>
       <c r="C61" t="str">
-        <v>1030513321</v>
+        <v>1030513130</v>
       </c>
       <c r="D61" t="str">
-        <v>葛亮</v>
+        <v>许鹏</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>林意</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B62" t="str">
-        <v>单色透明shader&amp;标准镜面高光shader</v>
+        <v>旅行社信息管理系统的设计与实现</v>
       </c>
       <c r="C62" t="str">
-        <v>1030513313</v>
+        <v>1030513205</v>
       </c>
       <c r="D62" t="str">
-        <v>倪晓琪</v>
+        <v>刘孟楠</v>
       </c>
     </row>
     <row r="63">
@@ -1247,139 +1247,139 @@
         <v>张得天</v>
       </c>
       <c r="B63" t="str">
-        <v>垂直爬虫开发</v>
+        <v>欺诈短信的数据挖掘</v>
       </c>
       <c r="C63" t="str">
-        <v>1030513332</v>
+        <v>1030513321</v>
       </c>
       <c r="D63" t="str">
-        <v>肖山民</v>
+        <v>葛亮</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>陈丽芳</v>
+        <v>谢振平</v>
       </c>
       <c r="B64" t="str">
-        <v>基于视频的目标识别与标记系统的研究与实现</v>
+        <v>基于监控视频的会展人流特征分析及可视化</v>
       </c>
       <c r="C64" t="str">
-        <v>1030513203</v>
+        <v>1030513429</v>
       </c>
       <c r="D64" t="str">
-        <v>李明泉</v>
+        <v>王伟林</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>孟磊</v>
+        <v>邓赵红</v>
       </c>
       <c r="B65" t="str">
-        <v>后工业语境下的数字技术与文化遗产整合应用方法探析</v>
+        <v>安卓平台人类特征识别软件开发</v>
       </c>
       <c r="C65" t="str">
-        <v>1030513202</v>
+        <v>1030513111</v>
       </c>
       <c r="D65" t="str">
-        <v>杜倩倩</v>
+        <v>龙仕清</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>谢振平</v>
+        <v>陈丽芳</v>
       </c>
       <c r="B66" t="str">
-        <v>大数据行为特征智能挖掘技术研究</v>
+        <v>基于视频的目标识别与标记系统的研究与实现</v>
       </c>
       <c r="C66" t="str">
-        <v>1030513101</v>
+        <v>1030513203</v>
       </c>
       <c r="D66" t="str">
-        <v>陈梅婕</v>
+        <v>李明泉</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>谢振平</v>
+        <v>林意</v>
       </c>
       <c r="B67" t="str">
-        <v>基于监控视频的会展人流特征分析及可视化</v>
+        <v>OpenCV边缘检测之比较</v>
       </c>
       <c r="C67" t="str">
-        <v>1030513429</v>
+        <v>1030513124</v>
       </c>
       <c r="D67" t="str">
-        <v>王伟林</v>
+        <v>刘家旺</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>邓赵红</v>
+        <v>晏涛</v>
       </c>
       <c r="B68" t="str">
-        <v>智能图像处理软件</v>
+        <v>本科毕业设计管理系统设计与实现</v>
       </c>
       <c r="C68" t="str">
-        <v>1030513431</v>
+        <v>1030513430</v>
       </c>
       <c r="D68" t="str">
-        <v>许嘉文</v>
+        <v>吴吉</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>陈秀宏</v>
+        <v>钱鹏江</v>
       </c>
       <c r="B69" t="str">
-        <v>3D虚拟文物展示</v>
+        <v>本科毕业设计管理系统设计与实现</v>
       </c>
       <c r="C69" t="str">
-        <v>1030513217</v>
+        <v>1030513425</v>
       </c>
       <c r="D69" t="str">
-        <v>张筱雨</v>
+        <v>郭震方</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>晏涛</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B70" t="str">
-        <v>立体图像匹配技术研究</v>
+        <v>基于Matlab的语音信号的采集与分析</v>
       </c>
       <c r="C70" t="str">
-        <v>1030513326</v>
+        <v>1030513118</v>
       </c>
       <c r="D70" t="str">
-        <v>苏德志</v>
+        <v>薛丹彤</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>丁彦蕊</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B71" t="str">
-        <v>大数据环境下的数据安全问题分析</v>
+        <v>基于智能方法的癫痫脑电信号识别研究</v>
       </c>
       <c r="C71" t="str">
-        <v>1030513318</v>
+        <v>1030513208</v>
       </c>
       <c r="D71" t="str">
-        <v>叶帼菁</v>
+        <v>卢虹羽</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>陈秀宏</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B72" t="str">
-        <v>基于VR技术的校园/景区漫游</v>
+        <v>基于Unity3D的VR项目设计与实现</v>
       </c>
       <c r="C72" t="str">
-        <v>1030513401</v>
+        <v>1030513413</v>
       </c>
       <c r="D72" t="str">
-        <v>蔡青</v>
+        <v>李越敏</v>
       </c>
     </row>
     <row r="73">
@@ -1387,55 +1387,55 @@
         <v>张得天</v>
       </c>
       <c r="B73" t="str">
-        <v>基于微信公众号的搜索平台设计与实现</v>
+        <v>Web前端开发</v>
       </c>
       <c r="C73" t="str">
-        <v>1030513325</v>
+        <v>1030513103</v>
       </c>
       <c r="D73" t="str">
-        <v>宋旭飞</v>
+        <v>甘姣姣</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>晏涛</v>
+        <v>蒋亦樟</v>
       </c>
       <c r="B74" t="str">
-        <v>多视点图像新视点生成技术研究</v>
+        <v>员工任务管理系统的设计与实现</v>
       </c>
       <c r="C74" t="str">
-        <v>1030513328</v>
+        <v>1030513104</v>
       </c>
       <c r="D74" t="str">
-        <v>王家麟</v>
+        <v>郭苹苹</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>孟磊</v>
+        <v>林意</v>
       </c>
       <c r="B75" t="str">
-        <v>基于移动互联模式改进非遗馆展项的系统开发与应用</v>
+        <v>OpenCV仿射变换与SURF特征点描述</v>
       </c>
       <c r="C75" t="str">
-        <v>1030513306</v>
+        <v>1030513223</v>
       </c>
       <c r="D75" t="str">
-        <v>李佳慧</v>
+        <v>李振明</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>蒋亦樟</v>
+        <v>晏涛</v>
       </c>
       <c r="B76" t="str">
-        <v>员工任务管理系统的设计与实现</v>
+        <v>立体图像匹配技术研究</v>
       </c>
       <c r="C76" t="str">
-        <v>1030513104</v>
+        <v>1030513326</v>
       </c>
       <c r="D76" t="str">
-        <v>郭苹苹</v>
+        <v>苏德志</v>
       </c>
     </row>
     <row r="77">
@@ -1443,69 +1443,69 @@
         <v>律睿敏</v>
       </c>
       <c r="B77" t="str">
-        <v>基于“六合棋”规则的解密类游戏开发</v>
+        <v>绘画解密游戏设计</v>
       </c>
       <c r="C77" t="str">
-        <v>1030513422</v>
+        <v>1030513122</v>
       </c>
       <c r="D77" t="str">
-        <v>白小山</v>
+        <v>金振阳</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>黄秋儒</v>
+        <v>晏涛</v>
       </c>
       <c r="B78" t="str">
-        <v>无锡地区非遗的数字化保护与传承（殷俊）</v>
+        <v>多视点图像新视点生成技术研究</v>
       </c>
       <c r="C78" t="str">
-        <v>1030513210</v>
+        <v>1030513328</v>
       </c>
       <c r="D78" t="str">
-        <v>田馨月</v>
+        <v>王家麟</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>蒋亦樟</v>
+        <v>张得天</v>
       </c>
       <c r="B79" t="str">
-        <v>面向甲状腺癌诊断的智能识别技术探索</v>
+        <v>基于企业数据的爬虫</v>
       </c>
       <c r="C79" t="str">
-        <v>1030513415</v>
+        <v>1030513129</v>
       </c>
       <c r="D79" t="str">
-        <v>刘英姿</v>
+        <v>王斌</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>晏涛</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B80" t="str">
-        <v>立体图像增强和自动编辑技术研究</v>
+        <v>基于虚拟现实技术的地方非遗保护程序设计</v>
       </c>
       <c r="C80" t="str">
-        <v>1030513324</v>
+        <v>1030513220</v>
       </c>
       <c r="D80" t="str">
-        <v>邱志强</v>
+        <v>朱雨婷</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>邓赵红</v>
+        <v>律睿敏</v>
       </c>
       <c r="B81" t="str">
-        <v>通用深度学习智能系统</v>
+        <v>基于“六合棋”规则的解密类游戏开发</v>
       </c>
       <c r="C81" t="str">
-        <v>1030513130</v>
+        <v>1030513422</v>
       </c>
       <c r="D81" t="str">
-        <v>许鹏</v>
+        <v>白小山</v>
       </c>
     </row>
     <row r="82">
@@ -1513,13 +1513,13 @@
         <v>陈秀宏</v>
       </c>
       <c r="B82" t="str">
-        <v>视频目标跟踪方法研究与实现</v>
+        <v>基于AR技术的手机游戏设计与开发</v>
       </c>
       <c r="C82" t="str">
-        <v>1030512302</v>
+        <v>1030513426</v>
       </c>
       <c r="D82" t="str">
-        <v>方旭</v>
+        <v>蒋子才</v>
       </c>
     </row>
     <row r="83">
@@ -1527,181 +1527,181 @@
         <v>黄秋儒</v>
       </c>
       <c r="B83" t="str">
-        <v>非遗语境下的博物馆交互性展示设计</v>
+        <v>无锡地区非遗的数字化保护与传承（殷俊）</v>
       </c>
       <c r="C83" t="str">
-        <v>1030513206</v>
+        <v>1030513210</v>
       </c>
       <c r="D83" t="str">
-        <v>刘楠</v>
+        <v>田馨月</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>林意</v>
+        <v>陈丽芳</v>
       </c>
       <c r="B84" t="str">
-        <v>OpenCV边缘检测之比较</v>
+        <v>基于压缩编码的数据隐藏算法的研究与实现</v>
       </c>
       <c r="C84" t="str">
-        <v>1030513124</v>
+        <v>1030513407</v>
       </c>
       <c r="D84" t="str">
-        <v>刘家旺</v>
+        <v>洪嘉惠</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>律睿敏</v>
+        <v>黄秋儒</v>
       </c>
       <c r="B85" t="str">
-        <v>“六合棋”的人机对战AI算法设计</v>
+        <v>医学教学视频中的3D转制应用与设计</v>
       </c>
       <c r="C85" t="str">
-        <v>1030513222</v>
+        <v>1030513106</v>
       </c>
       <c r="D85" t="str">
-        <v>李嘉文</v>
+        <v>贺东莉</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>张得天</v>
+        <v>钱鹏江</v>
       </c>
       <c r="B86" t="str">
-        <v>基于企业数据的爬虫</v>
+        <v>跨域知识学习技术及其在医学成像处理中的应用</v>
       </c>
       <c r="C86" t="str">
-        <v>1030513129</v>
+        <v>1030513320</v>
       </c>
       <c r="D86" t="str">
-        <v>王斌</v>
+        <v>郑佳敏</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>邓赵红</v>
+        <v>张得天</v>
       </c>
       <c r="B87" t="str">
-        <v>网络在线人类特征识别软件开发</v>
+        <v>微信公众号前端开发</v>
       </c>
       <c r="C87" t="str">
-        <v>1030513207</v>
+        <v>1030513112</v>
       </c>
       <c r="D87" t="str">
-        <v>刘思燚</v>
+        <v>毛姝婧</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>钱鹏江</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B88" t="str">
-        <v>本科毕业设计管理系统设计与实现</v>
+        <v>基于人眼虹膜识别的安防系统开发</v>
       </c>
       <c r="C88" t="str">
-        <v>1030513425</v>
+        <v>1030513102</v>
       </c>
       <c r="D88" t="str">
-        <v>郭震方</v>
+        <v>杜亚男</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>丁彦蕊</v>
+        <v>林意</v>
       </c>
       <c r="B89" t="str">
-        <v>基于3ds max的城市小区动画漫游设计与实现</v>
+        <v>基于Unity3D屏幕特效实现</v>
       </c>
       <c r="C89" t="str">
-        <v>1030513119</v>
+        <v>1030513412</v>
       </c>
       <c r="D89" t="str">
-        <v>姚陆吉</v>
+        <v>李诗芸</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>律睿敏</v>
+        <v>陈秀宏</v>
       </c>
       <c r="B90" t="str">
-        <v>具有音频编辑与分享功能的音乐播放器开发</v>
+        <v>图像特征与识别方法的研究与实现</v>
       </c>
       <c r="C90" t="str">
-        <v>1030513232</v>
+        <v>1030513128</v>
       </c>
       <c r="D90" t="str">
-        <v>杨笑寒</v>
+        <v>孙锐</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>陈丽芳</v>
+        <v>张得天</v>
       </c>
       <c r="B91" t="str">
-        <v>基于视频的目标计数与目标大小计算算法研究与实现</v>
+        <v>基于微信公众号的搜索平台设计与实现</v>
       </c>
       <c r="C91" t="str">
-        <v>1030513304</v>
+        <v>1030513325</v>
       </c>
       <c r="D91" t="str">
-        <v>贺怡</v>
+        <v>宋旭飞</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>林意</v>
+        <v>孟磊</v>
       </c>
       <c r="B92" t="str">
-        <v>OpenCV仿射变换与SURF特征点描述</v>
+        <v>后工业语境下的数字技术与文化遗产整合应用方法探析</v>
       </c>
       <c r="C92" t="str">
-        <v>1030513223</v>
+        <v>1030513202</v>
       </c>
       <c r="D92" t="str">
-        <v>李振明</v>
+        <v>杜倩倩</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>黄秋儒</v>
+        <v>孟磊</v>
       </c>
       <c r="B93" t="str">
-        <v>中国大陆新闻传播学学术文献数据库建设</v>
+        <v>基于移动互联模式改进非遗馆展项的系统开发与应用</v>
       </c>
       <c r="C93" t="str">
-        <v>1030513322</v>
+        <v>1030513306</v>
       </c>
       <c r="D93" t="str">
-        <v>郭晟</v>
+        <v>李佳慧</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>陈秀宏</v>
+        <v>律睿敏</v>
       </c>
       <c r="B94" t="str">
-        <v>图像特征与识别方法的研究与实现</v>
+        <v>一种新棋类游戏的故事化表现</v>
       </c>
       <c r="C94" t="str">
-        <v>1030513128</v>
+        <v>1030513424</v>
       </c>
       <c r="D94" t="str">
-        <v>孙锐</v>
+        <v>董天枢</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>张得天</v>
+        <v>谢振平</v>
       </c>
       <c r="B95" t="str">
-        <v>Web前端开发</v>
+        <v>食品安全动态数据的自动化采集与应用</v>
       </c>
       <c r="C95" t="str">
-        <v>1030513103</v>
+        <v>1030513428</v>
       </c>
       <c r="D95" t="str">
-        <v>甘姣姣</v>
+        <v>王涛</v>
       </c>
     </row>
     <row r="96">
@@ -1720,30 +1720,30 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>谢振平</v>
+        <v>丁彦蕊</v>
       </c>
       <c r="B97" t="str">
-        <v>食品安全动态数据的自动化采集与应用</v>
+        <v>基于微信的手游攻略平台设计</v>
       </c>
       <c r="C97" t="str">
-        <v>1030513428</v>
+        <v>1030513204</v>
       </c>
       <c r="D97" t="str">
-        <v>王涛</v>
+        <v>李韵芝</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>陈秀宏</v>
+        <v>晏涛</v>
       </c>
       <c r="B98" t="str">
-        <v>基于AR技术的手机游戏设计与开发</v>
+        <v>立体图像增强和自动编辑技术研究</v>
       </c>
       <c r="C98" t="str">
-        <v>1030513426</v>
+        <v>1030513324</v>
       </c>
       <c r="D98" t="str">
-        <v>蒋子才</v>
+        <v>邱志强</v>
       </c>
     </row>
   </sheetData>

</xml_diff>